<commit_message>
updated Fisher table with all entries
</commit_message>
<xml_diff>
--- a/results/Fishers_comparison.xlsx
+++ b/results/Fishers_comparison.xlsx
@@ -658,7 +658,9 @@
       <c r="C4" s="14" t="n">
         <v>0.3773962335319018</v>
       </c>
-      <c r="D4" s="14" t="n"/>
+      <c r="D4" s="14" t="n">
+        <v>9.919356917703732</v>
+      </c>
       <c r="E4" s="14" t="n">
         <v>4.689288745604718</v>
       </c>
@@ -675,7 +677,9 @@
       <c r="J4" s="14" t="n">
         <v>0.35284833961881</v>
       </c>
-      <c r="K4" s="14" t="n"/>
+      <c r="K4" s="14" t="n">
+        <v>4.304025912258477</v>
+      </c>
       <c r="L4" s="14" t="n">
         <v>4.689288745605105</v>
       </c>
@@ -704,7 +708,9 @@
         <v>0.3773962335319018</v>
       </c>
       <c r="C5" s="14" t="n"/>
-      <c r="D5" s="14" t="n"/>
+      <c r="D5" s="14" t="n">
+        <v>9.886936539789014</v>
+      </c>
       <c r="E5" s="14" t="n">
         <v>4.719477185936323</v>
       </c>
@@ -721,7 +727,9 @@
         <v>0.35284833961881</v>
       </c>
       <c r="J5" s="14" t="n"/>
-      <c r="K5" s="14" t="n"/>
+      <c r="K5" s="14" t="n">
+        <v>3.981254205101203</v>
+      </c>
       <c r="L5" s="14" t="n">
         <v>4.719477185933972</v>
       </c>
@@ -746,22 +754,38 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="B6" s="14" t="n"/>
-      <c r="C6" s="14" t="n"/>
+      <c r="B6" s="14" t="n">
+        <v>9.919356917703732</v>
+      </c>
+      <c r="C6" s="14" t="n">
+        <v>9.886936539789014</v>
+      </c>
       <c r="D6" s="14" t="n"/>
-      <c r="E6" s="14" t="n"/>
-      <c r="F6" s="14" t="n"/>
+      <c r="E6" s="14" t="n">
+        <v>7.117976427563766</v>
+      </c>
+      <c r="F6" s="14" t="n">
+        <v>9.99217094197501</v>
+      </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
         <is>
           <t>MP</t>
         </is>
       </c>
-      <c r="I6" s="14" t="n"/>
-      <c r="J6" s="14" t="n"/>
+      <c r="I6" s="14" t="n">
+        <v>4.304025912258477</v>
+      </c>
+      <c r="J6" s="14" t="n">
+        <v>3.981254205101203</v>
+      </c>
       <c r="K6" s="14" t="n"/>
-      <c r="L6" s="14" t="n"/>
-      <c r="M6" s="14" t="n"/>
+      <c r="L6" s="14" t="n">
+        <v>5.106398705457906</v>
+      </c>
+      <c r="M6" s="14" t="n">
+        <v>3.930611463694983</v>
+      </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
       <c r="P6" s="13" t="n"/>
@@ -786,7 +810,9 @@
       <c r="C7" s="14" t="n">
         <v>4.719477185936323</v>
       </c>
-      <c r="D7" s="14" t="n"/>
+      <c r="D7" s="14" t="n">
+        <v>7.117976427563766</v>
+      </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
         <v>4.708879397782754</v>
@@ -803,7 +829,9 @@
       <c r="J7" s="14" t="n">
         <v>4.719477185933972</v>
       </c>
-      <c r="K7" s="14" t="n"/>
+      <c r="K7" s="14" t="n">
+        <v>5.106398705457906</v>
+      </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
         <v>4.7088793977721</v>
@@ -832,7 +860,9 @@
       <c r="C8" s="14" t="n">
         <v>0.1761392290294239</v>
       </c>
-      <c r="D8" s="14" t="n"/>
+      <c r="D8" s="14" t="n">
+        <v>9.99217094197501</v>
+      </c>
       <c r="E8" s="14" t="n">
         <v>4.708879397782754</v>
       </c>
@@ -848,7 +878,9 @@
       <c r="J8" s="14" t="n">
         <v>0.2314736072303805</v>
       </c>
-      <c r="K8" s="14" t="n"/>
+      <c r="K8" s="14" t="n">
+        <v>3.930611463694983</v>
+      </c>
       <c r="L8" s="14" t="n">
         <v>4.7088793977721</v>
       </c>
@@ -962,7 +994,9 @@
       <c r="C14" s="14" t="n">
         <v>0.377396233533012</v>
       </c>
-      <c r="D14" s="14" t="n"/>
+      <c r="D14" s="14" t="n">
+        <v>9.919356917702338</v>
+      </c>
       <c r="E14" s="14" t="n">
         <v>3.186027703199337</v>
       </c>
@@ -978,7 +1012,9 @@
       <c r="J14" s="14" t="n">
         <v>0.002445764974182504</v>
       </c>
-      <c r="K14" s="14" t="n"/>
+      <c r="K14" s="14" t="n">
+        <v>4.264097540967208</v>
+      </c>
       <c r="L14" s="14" t="n">
         <v>0.005067295447965768</v>
       </c>
@@ -996,7 +1032,9 @@
         <v>0.377396233533012</v>
       </c>
       <c r="C15" s="14" t="n"/>
-      <c r="D15" s="14" t="n"/>
+      <c r="D15" s="14" t="n">
+        <v>9.886936539793002</v>
+      </c>
       <c r="E15" s="14" t="n">
         <v>3.15331911680175</v>
       </c>
@@ -1012,7 +1050,9 @@
         <v>0.002445764974182504</v>
       </c>
       <c r="J15" s="14" t="n"/>
-      <c r="K15" s="14" t="n"/>
+      <c r="K15" s="14" t="n">
+        <v>4.265870609220072</v>
+      </c>
       <c r="L15" s="14" t="n">
         <v>0.003617750813900871</v>
       </c>
@@ -1026,21 +1066,37 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="B16" s="14" t="n"/>
-      <c r="C16" s="14" t="n"/>
+      <c r="B16" s="14" t="n">
+        <v>9.919356917702338</v>
+      </c>
+      <c r="C16" s="14" t="n">
+        <v>9.886936539793002</v>
+      </c>
       <c r="D16" s="14" t="n"/>
-      <c r="E16" s="14" t="n"/>
-      <c r="F16" s="14" t="n"/>
+      <c r="E16" s="14" t="n">
+        <v>7.117976427563251</v>
+      </c>
+      <c r="F16" s="14" t="n">
+        <v>9.992170941966545</v>
+      </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
           <t>MP</t>
         </is>
       </c>
-      <c r="I16" s="14" t="n"/>
-      <c r="J16" s="14" t="n"/>
+      <c r="I16" s="14" t="n">
+        <v>4.264097540967208</v>
+      </c>
+      <c r="J16" s="14" t="n">
+        <v>4.265870609220072</v>
+      </c>
       <c r="K16" s="14" t="n"/>
-      <c r="L16" s="14" t="n"/>
-      <c r="M16" s="14" t="n"/>
+      <c r="L16" s="14" t="n">
+        <v>4.269155611861901</v>
+      </c>
+      <c r="M16" s="14" t="n">
+        <v>4.26838847448473</v>
+      </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
       <c r="A17" s="12" t="inlineStr">
@@ -1054,7 +1110,9 @@
       <c r="C17" s="14" t="n">
         <v>3.15331911680175</v>
       </c>
-      <c r="D17" s="14" t="n"/>
+      <c r="D17" s="14" t="n">
+        <v>7.117976427563251</v>
+      </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
         <v>3.259494281966406</v>
@@ -1070,7 +1128,9 @@
       <c r="J17" s="14" t="n">
         <v>0.003617750813900871</v>
       </c>
-      <c r="K17" s="14" t="n"/>
+      <c r="K17" s="14" t="n">
+        <v>4.269155611861901</v>
+      </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
         <v>0.001250791272115822</v>
@@ -1088,7 +1148,9 @@
       <c r="C18" s="14" t="n">
         <v>0.1761392290301824</v>
       </c>
-      <c r="D18" s="14" t="n"/>
+      <c r="D18" s="14" t="n">
+        <v>9.992170941966545</v>
+      </c>
       <c r="E18" s="14" t="n">
         <v>3.259494281966406</v>
       </c>
@@ -1104,7 +1166,9 @@
       <c r="J18" s="14" t="n">
         <v>0.002821980829311123</v>
       </c>
-      <c r="K18" s="14" t="n"/>
+      <c r="K18" s="14" t="n">
+        <v>4.26838847448473</v>
+      </c>
       <c r="L18" s="14" t="n">
         <v>0.001250791272115822</v>
       </c>
@@ -1302,7 +1366,9 @@
       <c r="C4" s="14" t="n">
         <v>0.3726463025137923</v>
       </c>
-      <c r="D4" s="14" t="n"/>
+      <c r="D4" s="14" t="n">
+        <v>10.84289138992081</v>
+      </c>
       <c r="E4" s="14" t="n">
         <v>1.173174098906264</v>
       </c>
@@ -1319,7 +1385,9 @@
       <c r="J4" s="14" t="n">
         <v>0.4491435128481215</v>
       </c>
-      <c r="K4" s="14" t="n"/>
+      <c r="K4" s="14" t="n">
+        <v>2.614010165875955</v>
+      </c>
       <c r="L4" s="14" t="n">
         <v>2.865230972178754</v>
       </c>
@@ -1348,7 +1416,9 @@
         <v>0.3726463025137923</v>
       </c>
       <c r="C5" s="14" t="n"/>
-      <c r="D5" s="14" t="n"/>
+      <c r="D5" s="14" t="n">
+        <v>10.8728026011959</v>
+      </c>
       <c r="E5" s="14" t="n">
         <v>1.314870456468473</v>
       </c>
@@ -1365,7 +1435,9 @@
         <v>0.4491435128481215</v>
       </c>
       <c r="J5" s="14" t="n"/>
-      <c r="K5" s="14" t="n"/>
+      <c r="K5" s="14" t="n">
+        <v>2.625541679111308</v>
+      </c>
       <c r="L5" s="14" t="n">
         <v>2.88437463456303</v>
       </c>
@@ -1390,22 +1462,38 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="B6" s="14" t="n"/>
-      <c r="C6" s="14" t="n"/>
+      <c r="B6" s="14" t="n">
+        <v>10.84289138992081</v>
+      </c>
+      <c r="C6" s="14" t="n">
+        <v>10.8728026011959</v>
+      </c>
       <c r="D6" s="14" t="n"/>
-      <c r="E6" s="14" t="n"/>
-      <c r="F6" s="14" t="n"/>
+      <c r="E6" s="14" t="n">
+        <v>10.5527857504133</v>
+      </c>
+      <c r="F6" s="14" t="n">
+        <v>10.84918233753177</v>
+      </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
         <is>
           <t>MP</t>
         </is>
       </c>
-      <c r="I6" s="14" t="n"/>
-      <c r="J6" s="14" t="n"/>
+      <c r="I6" s="14" t="n">
+        <v>2.614010165875955</v>
+      </c>
+      <c r="J6" s="14" t="n">
+        <v>2.625541679111308</v>
+      </c>
       <c r="K6" s="14" t="n"/>
-      <c r="L6" s="14" t="n"/>
-      <c r="M6" s="14" t="n"/>
+      <c r="L6" s="14" t="n">
+        <v>4.026938695190727</v>
+      </c>
+      <c r="M6" s="14" t="n">
+        <v>2.617148387586216</v>
+      </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
       <c r="P6" s="13" t="n"/>
@@ -1430,7 +1518,9 @@
       <c r="C7" s="14" t="n">
         <v>1.314870456468473</v>
       </c>
-      <c r="D7" s="14" t="n"/>
+      <c r="D7" s="14" t="n">
+        <v>10.5527857504133</v>
+      </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
         <v>1.260488548518442</v>
@@ -1447,7 +1537,9 @@
       <c r="J7" s="14" t="n">
         <v>2.88437463456303</v>
       </c>
-      <c r="K7" s="14" t="n"/>
+      <c r="K7" s="14" t="n">
+        <v>4.026938695190727</v>
+      </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
         <v>2.97560847582311</v>
@@ -1476,7 +1568,9 @@
       <c r="C8" s="14" t="n">
         <v>0.1081616267389053</v>
       </c>
-      <c r="D8" s="14" t="n"/>
+      <c r="D8" s="14" t="n">
+        <v>10.84918233753177</v>
+      </c>
       <c r="E8" s="14" t="n">
         <v>1.260488548518442</v>
       </c>
@@ -1492,7 +1586,9 @@
       <c r="J8" s="14" t="n">
         <v>0.1392586598233071</v>
       </c>
-      <c r="K8" s="14" t="n"/>
+      <c r="K8" s="14" t="n">
+        <v>2.617148387586216</v>
+      </c>
       <c r="L8" s="14" t="n">
         <v>2.97560847582311</v>
       </c>
@@ -1606,7 +1702,9 @@
       <c r="C14" s="14" t="n">
         <v>0.3726463025141316</v>
       </c>
-      <c r="D14" s="14" t="n"/>
+      <c r="D14" s="14" t="n">
+        <v>10.84289138992082</v>
+      </c>
       <c r="E14" s="14" t="n">
         <v>2.081437496736004</v>
       </c>
@@ -1622,7 +1720,9 @@
       <c r="J14" s="14" t="n">
         <v>0.004883347111689611</v>
       </c>
-      <c r="K14" s="14" t="n"/>
+      <c r="K14" s="14" t="n">
+        <v>3.453247927247328</v>
+      </c>
       <c r="L14" s="14" t="n">
         <v>0.005149342423874624</v>
       </c>
@@ -1640,7 +1740,9 @@
         <v>0.3726463025141316</v>
       </c>
       <c r="C15" s="14" t="n"/>
-      <c r="D15" s="14" t="n"/>
+      <c r="D15" s="14" t="n">
+        <v>10.87280260119602</v>
+      </c>
       <c r="E15" s="14" t="n">
         <v>2.106366134259678</v>
       </c>
@@ -1656,7 +1758,9 @@
         <v>0.004883347111689611</v>
       </c>
       <c r="J15" s="14" t="n"/>
-      <c r="K15" s="14" t="n"/>
+      <c r="K15" s="14" t="n">
+        <v>3.453996048594282</v>
+      </c>
       <c r="L15" s="14" t="n">
         <v>0.001263305374658307</v>
       </c>
@@ -1670,21 +1774,37 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="B16" s="14" t="n"/>
-      <c r="C16" s="14" t="n"/>
+      <c r="B16" s="14" t="n">
+        <v>10.84289138992082</v>
+      </c>
+      <c r="C16" s="14" t="n">
+        <v>10.87280260119602</v>
+      </c>
       <c r="D16" s="14" t="n"/>
-      <c r="E16" s="14" t="n"/>
-      <c r="F16" s="14" t="n"/>
+      <c r="E16" s="14" t="n">
+        <v>10.55278575041431</v>
+      </c>
+      <c r="F16" s="14" t="n">
+        <v>10.84918233753237</v>
+      </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
           <t>MP</t>
         </is>
       </c>
-      <c r="I16" s="14" t="n"/>
-      <c r="J16" s="14" t="n"/>
+      <c r="I16" s="14" t="n">
+        <v>3.453247927247328</v>
+      </c>
+      <c r="J16" s="14" t="n">
+        <v>3.453996048594282</v>
+      </c>
       <c r="K16" s="14" t="n"/>
-      <c r="L16" s="14" t="n"/>
-      <c r="M16" s="14" t="n"/>
+      <c r="L16" s="14" t="n">
+        <v>3.453945669386608</v>
+      </c>
+      <c r="M16" s="14" t="n">
+        <v>3.454313084573598</v>
+      </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
       <c r="A17" s="12" t="inlineStr">
@@ -1698,7 +1818,9 @@
       <c r="C17" s="14" t="n">
         <v>2.106366134259678</v>
       </c>
-      <c r="D17" s="14" t="n"/>
+      <c r="D17" s="14" t="n">
+        <v>10.55278575041431</v>
+      </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
         <v>2.104415939014535</v>
@@ -1714,7 +1836,9 @@
       <c r="J17" s="14" t="n">
         <v>0.001263305374658307</v>
       </c>
-      <c r="K17" s="14" t="n"/>
+      <c r="K17" s="14" t="n">
+        <v>3.453945669386608</v>
+      </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
         <v>0.001075452800861554</v>
@@ -1732,7 +1856,9 @@
       <c r="C18" s="14" t="n">
         <v>0.1081616267395801</v>
       </c>
-      <c r="D18" s="14" t="n"/>
+      <c r="D18" s="14" t="n">
+        <v>10.84918233753237</v>
+      </c>
       <c r="E18" s="14" t="n">
         <v>2.104415939014535</v>
       </c>
@@ -1748,7 +1874,9 @@
       <c r="J18" s="14" t="n">
         <v>0.001359305145372738</v>
       </c>
-      <c r="K18" s="14" t="n"/>
+      <c r="K18" s="14" t="n">
+        <v>3.454313084573598</v>
+      </c>
       <c r="L18" s="14" t="n">
         <v>0.001075452800861554</v>
       </c>
@@ -1946,7 +2074,9 @@
       <c r="C4" s="14" t="n">
         <v>0.2262904584537549</v>
       </c>
-      <c r="D4" s="14" t="n"/>
+      <c r="D4" s="14" t="n">
+        <v>9.041864007425653</v>
+      </c>
       <c r="E4" s="14" t="n">
         <v>2.701114701640339</v>
       </c>
@@ -1963,7 +2093,9 @@
       <c r="J4" s="14" t="n">
         <v>0.09070967271611728</v>
       </c>
-      <c r="K4" s="14" t="n"/>
+      <c r="K4" s="14" t="n">
+        <v>12.42479335229207</v>
+      </c>
       <c r="L4" s="14" t="n">
         <v>2.274282554125683</v>
       </c>
@@ -1992,7 +2124,9 @@
         <v>0.2262904584537549</v>
       </c>
       <c r="C5" s="14" t="n"/>
-      <c r="D5" s="14" t="n"/>
+      <c r="D5" s="14" t="n">
+        <v>9.073006014803994</v>
+      </c>
       <c r="E5" s="14" t="n">
         <v>2.844001213689403</v>
       </c>
@@ -2009,7 +2143,9 @@
         <v>0.09070967271611728</v>
       </c>
       <c r="J5" s="14" t="n"/>
-      <c r="K5" s="14" t="n"/>
+      <c r="K5" s="14" t="n">
+        <v>12.42567251460646</v>
+      </c>
       <c r="L5" s="14" t="n">
         <v>2.296414533926163</v>
       </c>
@@ -2034,22 +2170,38 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="B6" s="14" t="n"/>
-      <c r="C6" s="14" t="n"/>
+      <c r="B6" s="14" t="n">
+        <v>9.041864007425653</v>
+      </c>
+      <c r="C6" s="14" t="n">
+        <v>9.073006014803994</v>
+      </c>
       <c r="D6" s="14" t="n"/>
-      <c r="E6" s="14" t="n"/>
-      <c r="F6" s="14" t="n"/>
+      <c r="E6" s="14" t="n">
+        <v>9.703072181449262</v>
+      </c>
+      <c r="F6" s="14" t="n">
+        <v>8.960981046584797</v>
+      </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
         <is>
           <t>MP</t>
         </is>
       </c>
-      <c r="I6" s="14" t="n"/>
-      <c r="J6" s="14" t="n"/>
+      <c r="I6" s="14" t="n">
+        <v>12.42479335229207</v>
+      </c>
+      <c r="J6" s="14" t="n">
+        <v>12.42567251460646</v>
+      </c>
       <c r="K6" s="14" t="n"/>
-      <c r="L6" s="14" t="n"/>
-      <c r="M6" s="14" t="n"/>
+      <c r="L6" s="14" t="n">
+        <v>13.13783480376886</v>
+      </c>
+      <c r="M6" s="14" t="n">
+        <v>12.38050782994369</v>
+      </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
       <c r="P6" s="13" t="n"/>
@@ -2074,7 +2226,9 @@
       <c r="C7" s="14" t="n">
         <v>2.844001213689403</v>
       </c>
-      <c r="D7" s="14" t="n"/>
+      <c r="D7" s="14" t="n">
+        <v>9.703072181449262</v>
+      </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
         <v>2.72522560671845</v>
@@ -2091,7 +2245,9 @@
       <c r="J7" s="14" t="n">
         <v>2.296414533926163</v>
       </c>
-      <c r="K7" s="14" t="n"/>
+      <c r="K7" s="14" t="n">
+        <v>13.13783480376886</v>
+      </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
         <v>2.2572203961285</v>
@@ -2120,7 +2276,9 @@
       <c r="C8" s="14" t="n">
         <v>0.1309988390392303</v>
       </c>
-      <c r="D8" s="14" t="n"/>
+      <c r="D8" s="14" t="n">
+        <v>8.960981046584797</v>
+      </c>
       <c r="E8" s="14" t="n">
         <v>2.72522560671845</v>
       </c>
@@ -2136,7 +2294,9 @@
       <c r="J8" s="14" t="n">
         <v>0.1053254352962912</v>
       </c>
-      <c r="K8" s="14" t="n"/>
+      <c r="K8" s="14" t="n">
+        <v>12.38050782994369</v>
+      </c>
       <c r="L8" s="14" t="n">
         <v>2.2572203961285</v>
       </c>
@@ -2250,7 +2410,9 @@
       <c r="C14" s="14" t="n">
         <v>0.2262904584572695</v>
       </c>
-      <c r="D14" s="14" t="n"/>
+      <c r="D14" s="14" t="n">
+        <v>12.08381760429481</v>
+      </c>
       <c r="E14" s="14" t="n">
         <v>2.701114701647342</v>
       </c>
@@ -2266,7 +2428,9 @@
       <c r="J14" s="14" t="n">
         <v>0.009103929232176572</v>
       </c>
-      <c r="K14" s="14" t="n"/>
+      <c r="K14" s="14" t="n">
+        <v>0.474316134857282</v>
+      </c>
       <c r="L14" s="14" t="n">
         <v>0.005820922794185767</v>
       </c>
@@ -2284,7 +2448,9 @@
         <v>0.2262904584572695</v>
       </c>
       <c r="C15" s="14" t="n"/>
-      <c r="D15" s="14" t="n"/>
+      <c r="D15" s="14" t="n">
+        <v>12.04577796566226</v>
+      </c>
       <c r="E15" s="14" t="n">
         <v>2.844001213689614</v>
       </c>
@@ -2300,7 +2466,9 @@
         <v>0.009103929232176572</v>
       </c>
       <c r="J15" s="14" t="n"/>
-      <c r="K15" s="14" t="n"/>
+      <c r="K15" s="14" t="n">
+        <v>0.465363295794745</v>
+      </c>
       <c r="L15" s="14" t="n">
         <v>0.003367651523479847</v>
       </c>
@@ -2314,21 +2482,37 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="B16" s="14" t="n"/>
-      <c r="C16" s="14" t="n"/>
+      <c r="B16" s="14" t="n">
+        <v>12.08381760429481</v>
+      </c>
+      <c r="C16" s="14" t="n">
+        <v>12.04577796566226</v>
+      </c>
       <c r="D16" s="14" t="n"/>
-      <c r="E16" s="14" t="n"/>
-      <c r="F16" s="14" t="n"/>
+      <c r="E16" s="14" t="n">
+        <v>12.796691355624</v>
+      </c>
+      <c r="F16" s="14" t="n">
+        <v>12.09867764770548</v>
+      </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
           <t>MP</t>
         </is>
       </c>
-      <c r="I16" s="14" t="n"/>
-      <c r="J16" s="14" t="n"/>
+      <c r="I16" s="14" t="n">
+        <v>0.474316134857282</v>
+      </c>
+      <c r="J16" s="14" t="n">
+        <v>0.465363295794745</v>
+      </c>
       <c r="K16" s="14" t="n"/>
-      <c r="L16" s="14" t="n"/>
-      <c r="M16" s="14" t="n"/>
+      <c r="L16" s="14" t="n">
+        <v>0.4687308738595936</v>
+      </c>
+      <c r="M16" s="14" t="n">
+        <v>0.4701064277266727</v>
+      </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
       <c r="A17" s="12" t="inlineStr">
@@ -2342,7 +2526,9 @@
       <c r="C17" s="14" t="n">
         <v>2.844001213689614</v>
       </c>
-      <c r="D17" s="14" t="n"/>
+      <c r="D17" s="14" t="n">
+        <v>12.796691355624</v>
+      </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
         <v>2.725225606724025</v>
@@ -2358,7 +2544,9 @@
       <c r="J17" s="14" t="n">
         <v>0.003367651523479847</v>
       </c>
-      <c r="K17" s="14" t="n"/>
+      <c r="K17" s="14" t="n">
+        <v>0.4687308738595936</v>
+      </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
         <v>0.002265140801919659</v>
@@ -2376,7 +2564,9 @@
       <c r="C18" s="14" t="n">
         <v>0.1309988390130185</v>
       </c>
-      <c r="D18" s="14" t="n"/>
+      <c r="D18" s="14" t="n">
+        <v>12.09867764770548</v>
+      </c>
       <c r="E18" s="14" t="n">
         <v>2.725225606724025</v>
       </c>
@@ -2392,7 +2582,9 @@
       <c r="J18" s="14" t="n">
         <v>0.004743235699826326</v>
       </c>
-      <c r="K18" s="14" t="n"/>
+      <c r="K18" s="14" t="n">
+        <v>0.4701064277266727</v>
+      </c>
       <c r="L18" s="14" t="n">
         <v>0.002265140801919659</v>
       </c>
@@ -2590,7 +2782,9 @@
       <c r="C4" s="14" t="n">
         <v>0.06211140463036885</v>
       </c>
-      <c r="D4" s="14" t="n"/>
+      <c r="D4" s="14" t="n">
+        <v>8.062588612130609</v>
+      </c>
       <c r="E4" s="14" t="n">
         <v>2.874882720546051</v>
       </c>
@@ -2607,7 +2801,9 @@
       <c r="J4" s="14" t="n">
         <v>0.1030983777729827</v>
       </c>
-      <c r="K4" s="14" t="n"/>
+      <c r="K4" s="14" t="n">
+        <v>10.48676195248214</v>
+      </c>
       <c r="L4" s="14" t="n">
         <v>2.908151926234752</v>
       </c>
@@ -2636,7 +2832,9 @@
         <v>0.06211140463036885</v>
       </c>
       <c r="C5" s="14" t="n"/>
-      <c r="D5" s="14" t="n"/>
+      <c r="D5" s="14" t="n">
+        <v>8.006569333036184</v>
+      </c>
       <c r="E5" s="14" t="n">
         <v>2.935483613418856</v>
       </c>
@@ -2653,7 +2851,9 @@
         <v>0.1030983777729827</v>
       </c>
       <c r="J5" s="14" t="n"/>
-      <c r="K5" s="14" t="n"/>
+      <c r="K5" s="14" t="n">
+        <v>10.47856220274357</v>
+      </c>
       <c r="L5" s="14" t="n">
         <v>3.001984560012908</v>
       </c>
@@ -2678,22 +2878,38 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="B6" s="14" t="n"/>
-      <c r="C6" s="14" t="n"/>
+      <c r="B6" s="14" t="n">
+        <v>8.062588612130609</v>
+      </c>
+      <c r="C6" s="14" t="n">
+        <v>8.006569333036184</v>
+      </c>
       <c r="D6" s="14" t="n"/>
-      <c r="E6" s="14" t="n"/>
-      <c r="F6" s="14" t="n"/>
+      <c r="E6" s="14" t="n">
+        <v>8.856491601352039</v>
+      </c>
+      <c r="F6" s="14" t="n">
+        <v>7.859104476890197</v>
+      </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
         <is>
           <t>MP</t>
         </is>
       </c>
-      <c r="I6" s="14" t="n"/>
-      <c r="J6" s="14" t="n"/>
+      <c r="I6" s="14" t="n">
+        <v>10.48676195248214</v>
+      </c>
+      <c r="J6" s="14" t="n">
+        <v>10.47856220274357</v>
+      </c>
       <c r="K6" s="14" t="n"/>
-      <c r="L6" s="14" t="n"/>
-      <c r="M6" s="14" t="n"/>
+      <c r="L6" s="14" t="n">
+        <v>11.20511984687745</v>
+      </c>
+      <c r="M6" s="14" t="n">
+        <v>10.43795098231388</v>
+      </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
       <c r="P6" s="13" t="n"/>
@@ -2718,7 +2934,9 @@
       <c r="C7" s="14" t="n">
         <v>2.935483613418856</v>
       </c>
-      <c r="D7" s="14" t="n"/>
+      <c r="D7" s="14" t="n">
+        <v>8.856491601352039</v>
+      </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
         <v>2.749203952310937</v>
@@ -2735,7 +2953,9 @@
       <c r="J7" s="14" t="n">
         <v>3.001984560012908</v>
       </c>
-      <c r="K7" s="14" t="n"/>
+      <c r="K7" s="14" t="n">
+        <v>11.20511984687745</v>
+      </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
         <v>2.957255371749487</v>
@@ -2764,7 +2984,9 @@
       <c r="C8" s="14" t="n">
         <v>0.2263305621388694</v>
       </c>
-      <c r="D8" s="14" t="n"/>
+      <c r="D8" s="14" t="n">
+        <v>7.859104476890197</v>
+      </c>
       <c r="E8" s="14" t="n">
         <v>2.749203952310937</v>
       </c>
@@ -2780,7 +3002,9 @@
       <c r="J8" s="14" t="n">
         <v>0.0838425850827151</v>
       </c>
-      <c r="K8" s="14" t="n"/>
+      <c r="K8" s="14" t="n">
+        <v>10.43795098231388</v>
+      </c>
       <c r="L8" s="14" t="n">
         <v>2.957255371749487</v>
       </c>
@@ -2894,7 +3118,9 @@
       <c r="C14" s="14" t="n">
         <v>0.07873614082986091</v>
       </c>
-      <c r="D14" s="14" t="n"/>
+      <c r="D14" s="14" t="n">
+        <v>11.69423127716002</v>
+      </c>
       <c r="E14" s="14" t="n">
         <v>2.874882720540283</v>
       </c>
@@ -2910,7 +3136,9 @@
       <c r="J14" s="14" t="n">
         <v>0.009000578402860821</v>
       </c>
-      <c r="K14" s="14" t="n"/>
+      <c r="K14" s="14" t="n">
+        <v>0.3068155992074563</v>
+      </c>
       <c r="L14" s="14" t="n">
         <v>0.00584734573916154</v>
       </c>
@@ -2928,7 +3156,9 @@
         <v>0.07873614082986091</v>
       </c>
       <c r="C15" s="14" t="n"/>
-      <c r="D15" s="14" t="n"/>
+      <c r="D15" s="14" t="n">
+        <v>11.6573241284687</v>
+      </c>
       <c r="E15" s="14" t="n">
         <v>2.935483613414252</v>
       </c>
@@ -2944,7 +3174,9 @@
         <v>0.009000578402860821</v>
       </c>
       <c r="J15" s="14" t="n"/>
-      <c r="K15" s="14" t="n"/>
+      <c r="K15" s="14" t="n">
+        <v>0.2983315187058641</v>
+      </c>
       <c r="L15" s="14" t="n">
         <v>0.003200027864232041</v>
       </c>
@@ -2958,21 +3190,37 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="B16" s="14" t="n"/>
-      <c r="C16" s="14" t="n"/>
+      <c r="B16" s="14" t="n">
+        <v>11.69423127716002</v>
+      </c>
+      <c r="C16" s="14" t="n">
+        <v>11.6573241284687</v>
+      </c>
       <c r="D16" s="14" t="n"/>
-      <c r="E16" s="14" t="n"/>
-      <c r="F16" s="14" t="n"/>
+      <c r="E16" s="14" t="n">
+        <v>12.47793868942139</v>
+      </c>
+      <c r="F16" s="14" t="n">
+        <v>11.72636687679834</v>
+      </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
           <t>MP</t>
         </is>
       </c>
-      <c r="I16" s="14" t="n"/>
-      <c r="J16" s="14" t="n"/>
+      <c r="I16" s="14" t="n">
+        <v>0.3068155992074563</v>
+      </c>
+      <c r="J16" s="14" t="n">
+        <v>0.2983315187058641</v>
+      </c>
       <c r="K16" s="14" t="n"/>
-      <c r="L16" s="14" t="n"/>
-      <c r="M16" s="14" t="n"/>
+      <c r="L16" s="14" t="n">
+        <v>0.3011553713424278</v>
+      </c>
+      <c r="M16" s="14" t="n">
+        <v>0.3025150120135459</v>
+      </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
       <c r="A17" s="12" t="inlineStr">
@@ -2986,7 +3234,9 @@
       <c r="C17" s="14" t="n">
         <v>2.935483613414252</v>
       </c>
-      <c r="D17" s="14" t="n"/>
+      <c r="D17" s="14" t="n">
+        <v>12.47793868942139</v>
+      </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
         <v>2.749203952297027</v>
@@ -3002,7 +3252,9 @@
       <c r="J17" s="14" t="n">
         <v>0.003200027864232041</v>
       </c>
-      <c r="K17" s="14" t="n"/>
+      <c r="K17" s="14" t="n">
+        <v>0.3011553713424278</v>
+      </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
         <v>0.001997812498847041</v>
@@ -3020,7 +3272,9 @@
       <c r="C18" s="14" t="n">
         <v>0.2263305621488368</v>
       </c>
-      <c r="D18" s="14" t="n"/>
+      <c r="D18" s="14" t="n">
+        <v>11.72636687679834</v>
+      </c>
       <c r="E18" s="14" t="n">
         <v>2.749203952297027</v>
       </c>
@@ -3036,7 +3290,9 @@
       <c r="J18" s="14" t="n">
         <v>0.00418353106395057</v>
       </c>
-      <c r="K18" s="14" t="n"/>
+      <c r="K18" s="14" t="n">
+        <v>0.3025150120135459</v>
+      </c>
       <c r="L18" s="14" t="n">
         <v>0.001997812498847041</v>
       </c>

</xml_diff>

<commit_message>
updated fishers with w0 fixed
</commit_message>
<xml_diff>
--- a/results/Fishers_comparison.xlsx
+++ b/results/Fishers_comparison.xlsx
@@ -656,16 +656,16 @@
       </c>
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n">
-        <v>0.3773962335319018</v>
+        <v>0.3933583930807127</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>9.919356917703732</v>
+        <v>7.139904834961293</v>
       </c>
       <c r="E4" s="14" t="n">
-        <v>4.689288745604718</v>
+        <v>4.68928874560328</v>
       </c>
       <c r="F4" s="14" t="n">
-        <v>0.5485364935722695</v>
+        <v>0.5659270778387734</v>
       </c>
       <c r="G4" s="13" t="n"/>
       <c r="H4" s="12" t="inlineStr">
@@ -675,16 +675,16 @@
       </c>
       <c r="I4" s="14" t="n"/>
       <c r="J4" s="14" t="n">
-        <v>0.35284833961881</v>
+        <v>0.2914706440053519</v>
       </c>
       <c r="K4" s="14" t="n">
-        <v>4.304025912258477</v>
+        <v>0.918695872749776</v>
       </c>
       <c r="L4" s="14" t="n">
-        <v>4.689288745605105</v>
+        <v>4.689288745603631</v>
       </c>
       <c r="M4" s="14" t="n">
-        <v>0.5518494451161595</v>
+        <v>0.5520209231003159</v>
       </c>
       <c r="N4" s="13" t="n"/>
       <c r="O4" s="13" t="n"/>
@@ -705,17 +705,17 @@
         </is>
       </c>
       <c r="B5" s="14" t="n">
-        <v>0.3773962335319018</v>
+        <v>0.3933583930807127</v>
       </c>
       <c r="C5" s="14" t="n"/>
       <c r="D5" s="14" t="n">
-        <v>9.886936539789014</v>
+        <v>7.132839771095703</v>
       </c>
       <c r="E5" s="14" t="n">
-        <v>4.719477185936323</v>
+        <v>4.719477185931866</v>
       </c>
       <c r="F5" s="14" t="n">
-        <v>0.1761392290294239</v>
+        <v>0.1725725264324497</v>
       </c>
       <c r="G5" s="13" t="n"/>
       <c r="H5" s="12" t="inlineStr">
@@ -724,17 +724,17 @@
         </is>
       </c>
       <c r="I5" s="14" t="n">
-        <v>0.35284833961881</v>
+        <v>0.2914706440053519</v>
       </c>
       <c r="J5" s="14" t="n"/>
       <c r="K5" s="14" t="n">
-        <v>3.981254205101203</v>
+        <v>1.025702549209454</v>
       </c>
       <c r="L5" s="14" t="n">
-        <v>4.719477185933972</v>
+        <v>4.719477185932573</v>
       </c>
       <c r="M5" s="14" t="n">
-        <v>0.2314736072303805</v>
+        <v>0.2709135937613568</v>
       </c>
       <c r="N5" s="13" t="n"/>
       <c r="O5" s="13" t="n"/>
@@ -755,17 +755,17 @@
         </is>
       </c>
       <c r="B6" s="14" t="n">
-        <v>9.919356917703732</v>
+        <v>7.139904834961293</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>9.886936539789014</v>
+        <v>7.132839771095703</v>
       </c>
       <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n">
-        <v>7.117976427563766</v>
+        <v>7.162434942445494</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>9.99217094197501</v>
+        <v>7.146058268680489</v>
       </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
@@ -774,17 +774,17 @@
         </is>
       </c>
       <c r="I6" s="14" t="n">
-        <v>4.304025912258477</v>
+        <v>0.918695872749776</v>
       </c>
       <c r="J6" s="14" t="n">
-        <v>3.981254205101203</v>
+        <v>1.025702549209454</v>
       </c>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n">
-        <v>5.106398705457906</v>
+        <v>5.106398705459438</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>3.930611463694983</v>
+        <v>1.286222646092567</v>
       </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
@@ -805,17 +805,17 @@
         </is>
       </c>
       <c r="B7" s="14" t="n">
-        <v>4.689288745604718</v>
+        <v>4.68928874560328</v>
       </c>
       <c r="C7" s="14" t="n">
-        <v>4.719477185936323</v>
+        <v>4.719477185931866</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>7.117976427563766</v>
+        <v>7.162434942445494</v>
       </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
-        <v>4.708879397782754</v>
+        <v>4.708879397770238</v>
       </c>
       <c r="G7" s="13" t="n"/>
       <c r="H7" s="12" t="inlineStr">
@@ -824,17 +824,17 @@
         </is>
       </c>
       <c r="I7" s="14" t="n">
-        <v>4.689288745605105</v>
+        <v>4.689288745603631</v>
       </c>
       <c r="J7" s="14" t="n">
-        <v>4.719477185933972</v>
+        <v>4.719477185932573</v>
       </c>
       <c r="K7" s="14" t="n">
-        <v>5.106398705457906</v>
+        <v>5.106398705459438</v>
       </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
-        <v>4.7088793977721</v>
+        <v>4.708879397770369</v>
       </c>
       <c r="N7" s="13" t="n"/>
       <c r="O7" s="13" t="n"/>
@@ -855,16 +855,16 @@
         </is>
       </c>
       <c r="B8" s="14" t="n">
-        <v>0.5485364935722695</v>
+        <v>0.5659270778387734</v>
       </c>
       <c r="C8" s="14" t="n">
-        <v>0.1761392290294239</v>
+        <v>0.1725725264324497</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>9.99217094197501</v>
+        <v>7.146058268680489</v>
       </c>
       <c r="E8" s="14" t="n">
-        <v>4.708879397782754</v>
+        <v>4.708879397770238</v>
       </c>
       <c r="F8" s="14" t="n"/>
       <c r="H8" s="12" t="inlineStr">
@@ -873,16 +873,16 @@
         </is>
       </c>
       <c r="I8" s="14" t="n">
-        <v>0.5518494451161595</v>
+        <v>0.5520209231003159</v>
       </c>
       <c r="J8" s="14" t="n">
-        <v>0.2314736072303805</v>
+        <v>0.2709135937613568</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>3.930611463694983</v>
+        <v>1.286222646092567</v>
       </c>
       <c r="L8" s="14" t="n">
-        <v>4.7088793977721</v>
+        <v>4.708879397770369</v>
       </c>
       <c r="M8" s="14" t="n"/>
     </row>
@@ -992,16 +992,16 @@
       </c>
       <c r="B14" s="14" t="n"/>
       <c r="C14" s="14" t="n">
-        <v>0.377396233533012</v>
+        <v>0.3933583930822886</v>
       </c>
       <c r="D14" s="14" t="n">
-        <v>9.919356917702338</v>
+        <v>7.139904834960271</v>
       </c>
       <c r="E14" s="14" t="n">
-        <v>3.186027703199337</v>
+        <v>1.829972646983461</v>
       </c>
       <c r="F14" s="14" t="n">
-        <v>0.5485364935734055</v>
+        <v>0.5659270778406734</v>
       </c>
       <c r="H14" s="12" t="inlineStr">
         <is>
@@ -1013,13 +1013,13 @@
         <v>0.002445764974182504</v>
       </c>
       <c r="K14" s="14" t="n">
-        <v>4.264097540967208</v>
+        <v>4.264097540967207</v>
       </c>
       <c r="L14" s="14" t="n">
-        <v>0.005067295447965768</v>
+        <v>0.005067295447945582</v>
       </c>
       <c r="M14" s="14" t="n">
-        <v>0.004494523199528501</v>
+        <v>0.004494523199528502</v>
       </c>
     </row>
     <row r="15" ht="15.85" customHeight="1" s="10">
@@ -1029,17 +1029,17 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0.377396233533012</v>
+        <v>0.3933583930822886</v>
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n">
-        <v>9.886936539793002</v>
+        <v>7.132839771094387</v>
       </c>
       <c r="E15" s="14" t="n">
-        <v>3.15331911680175</v>
+        <v>1.869822266392103</v>
       </c>
       <c r="F15" s="14" t="n">
-        <v>0.1761392290301824</v>
+        <v>0.1725725264327739</v>
       </c>
       <c r="H15" s="12" t="inlineStr">
         <is>
@@ -1051,13 +1051,13 @@
       </c>
       <c r="J15" s="14" t="n"/>
       <c r="K15" s="14" t="n">
-        <v>4.265870609220072</v>
+        <v>4.265870609220071</v>
       </c>
       <c r="L15" s="14" t="n">
-        <v>0.003617750813900871</v>
+        <v>0.003617750813871641</v>
       </c>
       <c r="M15" s="14" t="n">
-        <v>0.002821980829311123</v>
+        <v>0.002821980829281891</v>
       </c>
     </row>
     <row r="16" ht="15.85" customHeight="1" s="10">
@@ -1067,17 +1067,17 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>9.919356917702338</v>
+        <v>7.139904834960271</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>9.886936539793002</v>
+        <v>7.132839771094387</v>
       </c>
       <c r="D16" s="14" t="n"/>
       <c r="E16" s="14" t="n">
-        <v>7.117976427563251</v>
+        <v>7.162434942443958</v>
       </c>
       <c r="F16" s="14" t="n">
-        <v>9.992170941966545</v>
+        <v>7.146058268680336</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
@@ -1085,17 +1085,17 @@
         </is>
       </c>
       <c r="I16" s="14" t="n">
-        <v>4.264097540967208</v>
+        <v>4.264097540967207</v>
       </c>
       <c r="J16" s="14" t="n">
-        <v>4.265870609220072</v>
+        <v>4.265870609220071</v>
       </c>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n">
-        <v>4.269155611861901</v>
+        <v>4.2691556118619</v>
       </c>
       <c r="M16" s="14" t="n">
-        <v>4.26838847448473</v>
+        <v>4.268388474484729</v>
       </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
@@ -1105,17 +1105,17 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>3.186027703199337</v>
+        <v>1.829972646983461</v>
       </c>
       <c r="C17" s="14" t="n">
-        <v>3.15331911680175</v>
+        <v>1.869822266392103</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>7.117976427563251</v>
+        <v>7.162434942443958</v>
       </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
-        <v>3.259494281966406</v>
+        <v>1.869051833068244</v>
       </c>
       <c r="H17" s="12" t="inlineStr">
         <is>
@@ -1123,17 +1123,17 @@
         </is>
       </c>
       <c r="I17" s="14" t="n">
-        <v>0.005067295447965768</v>
+        <v>0.005067295447945582</v>
       </c>
       <c r="J17" s="14" t="n">
-        <v>0.003617750813900871</v>
+        <v>0.003617750813871641</v>
       </c>
       <c r="K17" s="14" t="n">
-        <v>4.269155611861901</v>
+        <v>4.2691556118619</v>
       </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
-        <v>0.001250791272115822</v>
+        <v>0.001250791272543508</v>
       </c>
     </row>
     <row r="18" ht="15.85" customHeight="1" s="10">
@@ -1143,16 +1143,16 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0.5485364935734055</v>
+        <v>0.5659270778406734</v>
       </c>
       <c r="C18" s="14" t="n">
-        <v>0.1761392290301824</v>
+        <v>0.1725725264327739</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>9.992170941966545</v>
+        <v>7.146058268680336</v>
       </c>
       <c r="E18" s="14" t="n">
-        <v>3.259494281966406</v>
+        <v>1.869051833068244</v>
       </c>
       <c r="F18" s="14" t="n"/>
       <c r="H18" s="12" t="inlineStr">
@@ -1161,16 +1161,16 @@
         </is>
       </c>
       <c r="I18" s="14" t="n">
-        <v>0.004494523199528501</v>
+        <v>0.004494523199528502</v>
       </c>
       <c r="J18" s="14" t="n">
-        <v>0.002821980829311123</v>
+        <v>0.002821980829281891</v>
       </c>
       <c r="K18" s="14" t="n">
-        <v>4.26838847448473</v>
+        <v>4.268388474484729</v>
       </c>
       <c r="L18" s="14" t="n">
-        <v>0.001250791272115822</v>
+        <v>0.001250791272543508</v>
       </c>
       <c r="M18" s="14" t="n"/>
     </row>
@@ -1364,16 +1364,16 @@
       </c>
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n">
-        <v>0.3726463025137923</v>
+        <v>0.3882526983703625</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>10.84289138992081</v>
+        <v>3.430285859195056</v>
       </c>
       <c r="E4" s="14" t="n">
-        <v>1.173174098906264</v>
+        <v>1.064506527562792</v>
       </c>
       <c r="F4" s="14" t="n">
-        <v>0.4808059913145969</v>
+        <v>0.4888362339453383</v>
       </c>
       <c r="G4" s="13" t="n"/>
       <c r="H4" s="12" t="inlineStr">
@@ -1383,16 +1383,16 @@
       </c>
       <c r="I4" s="14" t="n"/>
       <c r="J4" s="14" t="n">
-        <v>0.4491435128481215</v>
+        <v>0.449960705173272</v>
       </c>
       <c r="K4" s="14" t="n">
-        <v>2.614010165875955</v>
+        <v>1.037021323985908</v>
       </c>
       <c r="L4" s="14" t="n">
-        <v>2.865230972178754</v>
+        <v>1.983452788096468</v>
       </c>
       <c r="M4" s="14" t="n">
-        <v>0.5774622991955048</v>
+        <v>0.5931752521592301</v>
       </c>
       <c r="N4" s="13" t="n"/>
       <c r="O4" s="13" t="n"/>
@@ -1413,17 +1413,17 @@
         </is>
       </c>
       <c r="B5" s="14" t="n">
-        <v>0.3726463025137923</v>
+        <v>0.3882526983703625</v>
       </c>
       <c r="C5" s="14" t="n"/>
       <c r="D5" s="14" t="n">
-        <v>10.8728026011959</v>
+        <v>3.43095438582424</v>
       </c>
       <c r="E5" s="14" t="n">
-        <v>1.314870456468473</v>
+        <v>1.236509068301738</v>
       </c>
       <c r="F5" s="14" t="n">
-        <v>0.1081616267389053</v>
+        <v>0.1144918060678667</v>
       </c>
       <c r="G5" s="13" t="n"/>
       <c r="H5" s="12" t="inlineStr">
@@ -1432,17 +1432,17 @@
         </is>
       </c>
       <c r="I5" s="14" t="n">
-        <v>0.4491435128481215</v>
+        <v>0.449960705173272</v>
       </c>
       <c r="J5" s="14" t="n"/>
       <c r="K5" s="14" t="n">
-        <v>2.625541679111308</v>
+        <v>1.03616913080369</v>
       </c>
       <c r="L5" s="14" t="n">
-        <v>2.88437463456303</v>
+        <v>1.930243695889936</v>
       </c>
       <c r="M5" s="14" t="n">
-        <v>0.1392586598233071</v>
+        <v>0.143218369563796</v>
       </c>
       <c r="N5" s="13" t="n"/>
       <c r="O5" s="13" t="n"/>
@@ -1463,17 +1463,17 @@
         </is>
       </c>
       <c r="B6" s="14" t="n">
-        <v>10.84289138992081</v>
+        <v>3.430285859195056</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>10.8728026011959</v>
+        <v>3.43095438582424</v>
       </c>
       <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n">
-        <v>10.5527857504133</v>
+        <v>3.430929996969808</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>10.84918233753177</v>
+        <v>3.43124230468613</v>
       </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
@@ -1482,17 +1482,17 @@
         </is>
       </c>
       <c r="I6" s="14" t="n">
-        <v>2.614010165875955</v>
+        <v>1.037021323985908</v>
       </c>
       <c r="J6" s="14" t="n">
-        <v>2.625541679111308</v>
+        <v>1.03616913080369</v>
       </c>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n">
-        <v>4.026938695190727</v>
+        <v>1.163057864852788</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>2.617148387586216</v>
+        <v>1.041473410754264</v>
       </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
@@ -1513,17 +1513,17 @@
         </is>
       </c>
       <c r="B7" s="14" t="n">
-        <v>1.173174098906264</v>
+        <v>1.064506527562792</v>
       </c>
       <c r="C7" s="14" t="n">
-        <v>1.314870456468473</v>
+        <v>1.236509068301738</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>10.5527857504133</v>
+        <v>3.430929996969808</v>
       </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
-        <v>1.260488548518442</v>
+        <v>1.176756642942559</v>
       </c>
       <c r="G7" s="13" t="n"/>
       <c r="H7" s="12" t="inlineStr">
@@ -1532,17 +1532,17 @@
         </is>
       </c>
       <c r="I7" s="14" t="n">
-        <v>2.865230972178754</v>
+        <v>1.983452788096468</v>
       </c>
       <c r="J7" s="14" t="n">
-        <v>2.88437463456303</v>
+        <v>1.930243695889936</v>
       </c>
       <c r="K7" s="14" t="n">
-        <v>4.026938695190727</v>
+        <v>1.163057864852788</v>
       </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
-        <v>2.97560847582311</v>
+        <v>1.975326851707516</v>
       </c>
       <c r="N7" s="13" t="n"/>
       <c r="O7" s="13" t="n"/>
@@ -1563,16 +1563,16 @@
         </is>
       </c>
       <c r="B8" s="14" t="n">
-        <v>0.4808059913145969</v>
+        <v>0.4888362339453383</v>
       </c>
       <c r="C8" s="14" t="n">
-        <v>0.1081616267389053</v>
+        <v>0.1144918060678667</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>10.84918233753177</v>
+        <v>3.43124230468613</v>
       </c>
       <c r="E8" s="14" t="n">
-        <v>1.260488548518442</v>
+        <v>1.176756642942559</v>
       </c>
       <c r="F8" s="14" t="n"/>
       <c r="H8" s="12" t="inlineStr">
@@ -1581,16 +1581,16 @@
         </is>
       </c>
       <c r="I8" s="14" t="n">
-        <v>0.5774622991955048</v>
+        <v>0.5931752521592301</v>
       </c>
       <c r="J8" s="14" t="n">
-        <v>0.1392586598233071</v>
+        <v>0.143218369563796</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>2.617148387586216</v>
+        <v>1.041473410754264</v>
       </c>
       <c r="L8" s="14" t="n">
-        <v>2.97560847582311</v>
+        <v>1.975326851707516</v>
       </c>
       <c r="M8" s="14" t="n"/>
     </row>
@@ -1700,16 +1700,16 @@
       </c>
       <c r="B14" s="14" t="n"/>
       <c r="C14" s="14" t="n">
-        <v>0.3726463025141316</v>
+        <v>0.3882526983701607</v>
       </c>
       <c r="D14" s="14" t="n">
-        <v>10.84289138992082</v>
+        <v>3.290434336662218</v>
       </c>
       <c r="E14" s="14" t="n">
-        <v>2.081437496736004</v>
+        <v>2.08143749673649</v>
       </c>
       <c r="F14" s="14" t="n">
-        <v>0.4808059913156109</v>
+        <v>0.4888362339462129</v>
       </c>
       <c r="H14" s="12" t="inlineStr">
         <is>
@@ -1718,16 +1718,16 @@
       </c>
       <c r="I14" s="14" t="n"/>
       <c r="J14" s="14" t="n">
-        <v>0.004883347111689611</v>
+        <v>0.004883347111208501</v>
       </c>
       <c r="K14" s="14" t="n">
-        <v>3.453247927247328</v>
+        <v>3.453247927247299</v>
       </c>
       <c r="L14" s="14" t="n">
-        <v>0.005149342423874624</v>
+        <v>0.005149342424232372</v>
       </c>
       <c r="M14" s="14" t="n">
-        <v>0.006224795222596624</v>
+        <v>0.006224795222325194</v>
       </c>
     </row>
     <row r="15" ht="15.85" customHeight="1" s="10">
@@ -1737,17 +1737,17 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0.3726463025141316</v>
+        <v>0.3882526983701607</v>
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n">
-        <v>10.87280260119602</v>
+        <v>3.303424191205476</v>
       </c>
       <c r="E15" s="14" t="n">
-        <v>2.106366134259678</v>
+        <v>2.106366134259916</v>
       </c>
       <c r="F15" s="14" t="n">
-        <v>0.1081616267395801</v>
+        <v>0.1144918060680573</v>
       </c>
       <c r="H15" s="12" t="inlineStr">
         <is>
@@ -1755,17 +1755,17 @@
         </is>
       </c>
       <c r="I15" s="14" t="n">
-        <v>0.004883347111689611</v>
+        <v>0.004883347111208501</v>
       </c>
       <c r="J15" s="14" t="n"/>
       <c r="K15" s="14" t="n">
-        <v>3.453996048594282</v>
+        <v>3.453996048594386</v>
       </c>
       <c r="L15" s="14" t="n">
         <v>0.001263305374658307</v>
       </c>
       <c r="M15" s="14" t="n">
-        <v>0.001359305145372738</v>
+        <v>0.001359305144591694</v>
       </c>
     </row>
     <row r="16" ht="15.85" customHeight="1" s="10">
@@ -1775,17 +1775,17 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>10.84289138992082</v>
+        <v>3.290434336662218</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>10.87280260119602</v>
+        <v>3.303424191205476</v>
       </c>
       <c r="D16" s="14" t="n"/>
       <c r="E16" s="14" t="n">
-        <v>10.55278575041431</v>
+        <v>3.177144852113471</v>
       </c>
       <c r="F16" s="14" t="n">
-        <v>10.84918233753237</v>
+        <v>3.284614487142579</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
@@ -1793,17 +1793,17 @@
         </is>
       </c>
       <c r="I16" s="14" t="n">
-        <v>3.453247927247328</v>
+        <v>3.453247927247299</v>
       </c>
       <c r="J16" s="14" t="n">
-        <v>3.453996048594282</v>
+        <v>3.453996048594386</v>
       </c>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n">
-        <v>3.453945669386608</v>
+        <v>3.453945669386594</v>
       </c>
       <c r="M16" s="14" t="n">
-        <v>3.454313084573598</v>
+        <v>3.454313084573613</v>
       </c>
     </row>
     <row r="17" ht="15.85" customHeight="1" s="10">
@@ -1813,17 +1813,17 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>2.081437496736004</v>
+        <v>2.08143749673649</v>
       </c>
       <c r="C17" s="14" t="n">
-        <v>2.106366134259678</v>
+        <v>2.106366134259916</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>10.55278575041431</v>
+        <v>3.177144852113471</v>
       </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
-        <v>2.104415939014535</v>
+        <v>2.104415939014608</v>
       </c>
       <c r="H17" s="12" t="inlineStr">
         <is>
@@ -1831,17 +1831,17 @@
         </is>
       </c>
       <c r="I17" s="14" t="n">
-        <v>0.005149342423874624</v>
+        <v>0.005149342424232372</v>
       </c>
       <c r="J17" s="14" t="n">
         <v>0.001263305374658307</v>
       </c>
       <c r="K17" s="14" t="n">
-        <v>3.453945669386608</v>
+        <v>3.453945669386594</v>
       </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
-        <v>0.001075452800861554</v>
+        <v>0.001075452800553141</v>
       </c>
     </row>
     <row r="18" ht="15.85" customHeight="1" s="10">
@@ -1851,16 +1851,16 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0.4808059913156109</v>
+        <v>0.4888362339462129</v>
       </c>
       <c r="C18" s="14" t="n">
-        <v>0.1081616267395801</v>
+        <v>0.1144918060680573</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>10.84918233753237</v>
+        <v>3.284614487142579</v>
       </c>
       <c r="E18" s="14" t="n">
-        <v>2.104415939014535</v>
+        <v>2.104415939014608</v>
       </c>
       <c r="F18" s="14" t="n"/>
       <c r="H18" s="12" t="inlineStr">
@@ -1869,16 +1869,16 @@
         </is>
       </c>
       <c r="I18" s="14" t="n">
-        <v>0.006224795222596624</v>
+        <v>0.006224795222325194</v>
       </c>
       <c r="J18" s="14" t="n">
-        <v>0.001359305145372738</v>
+        <v>0.001359305144591694</v>
       </c>
       <c r="K18" s="14" t="n">
-        <v>3.454313084573598</v>
+        <v>3.454313084573613</v>
       </c>
       <c r="L18" s="14" t="n">
-        <v>0.001075452800861554</v>
+        <v>0.001075452800553141</v>
       </c>
       <c r="M18" s="14" t="n"/>
     </row>
@@ -2072,16 +2072,16 @@
       </c>
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n">
-        <v>0.2262904584537549</v>
+        <v>0.142449201371621</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>9.041864007425653</v>
+        <v>8.630162378114971</v>
       </c>
       <c r="E4" s="14" t="n">
-        <v>2.701114701640339</v>
+        <v>1.038669115503516</v>
       </c>
       <c r="F4" s="14" t="n">
-        <v>0.1144526964760178</v>
+        <v>0.2282711709727175</v>
       </c>
       <c r="G4" s="13" t="n"/>
       <c r="H4" s="12" t="inlineStr">
@@ -2091,16 +2091,16 @@
       </c>
       <c r="I4" s="14" t="n"/>
       <c r="J4" s="14" t="n">
-        <v>0.09070967271611728</v>
+        <v>0.1470639756132987</v>
       </c>
       <c r="K4" s="14" t="n">
-        <v>12.42479335229207</v>
+        <v>6.051617533267599</v>
       </c>
       <c r="L4" s="14" t="n">
-        <v>2.274282554125683</v>
+        <v>0.4963982727724712</v>
       </c>
       <c r="M4" s="14" t="n">
-        <v>0.1960349207199441</v>
+        <v>0.2444829367845394</v>
       </c>
       <c r="N4" s="13" t="n"/>
       <c r="O4" s="13" t="n"/>
@@ -2121,17 +2121,17 @@
         </is>
       </c>
       <c r="B5" s="14" t="n">
-        <v>0.2262904584537549</v>
+        <v>0.142449201371621</v>
       </c>
       <c r="C5" s="14" t="n"/>
       <c r="D5" s="14" t="n">
-        <v>9.073006014803994</v>
+        <v>8.688459101732617</v>
       </c>
       <c r="E5" s="14" t="n">
-        <v>2.844001213689403</v>
+        <v>1.073222713296864</v>
       </c>
       <c r="F5" s="14" t="n">
-        <v>0.1309988390392303</v>
+        <v>0.1043430787734386</v>
       </c>
       <c r="G5" s="13" t="n"/>
       <c r="H5" s="12" t="inlineStr">
@@ -2140,17 +2140,17 @@
         </is>
       </c>
       <c r="I5" s="14" t="n">
-        <v>0.09070967271611728</v>
+        <v>0.1470639756132987</v>
       </c>
       <c r="J5" s="14" t="n"/>
       <c r="K5" s="14" t="n">
-        <v>12.42567251460646</v>
+        <v>6.073385649353082</v>
       </c>
       <c r="L5" s="14" t="n">
-        <v>2.296414533926163</v>
+        <v>0.5128299628413603</v>
       </c>
       <c r="M5" s="14" t="n">
-        <v>0.1053254352962912</v>
+        <v>0.09741931143881596</v>
       </c>
       <c r="N5" s="13" t="n"/>
       <c r="O5" s="13" t="n"/>
@@ -2171,17 +2171,17 @@
         </is>
       </c>
       <c r="B6" s="14" t="n">
-        <v>9.041864007425653</v>
+        <v>8.630162378114971</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>9.073006014803994</v>
+        <v>8.688459101732617</v>
       </c>
       <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n">
-        <v>9.703072181449262</v>
+        <v>8.001189077243545</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>8.960981046584797</v>
+        <v>8.670575811054526</v>
       </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
@@ -2190,17 +2190,17 @@
         </is>
       </c>
       <c r="I6" s="14" t="n">
-        <v>12.42479335229207</v>
+        <v>6.051617533267599</v>
       </c>
       <c r="J6" s="14" t="n">
-        <v>12.42567251460646</v>
+        <v>6.073385649353082</v>
       </c>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n">
-        <v>13.13783480376886</v>
+        <v>6.242689743567973</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>12.38050782994369</v>
+        <v>6.057376353151263</v>
       </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
@@ -2221,17 +2221,17 @@
         </is>
       </c>
       <c r="B7" s="14" t="n">
-        <v>2.701114701640339</v>
+        <v>1.038669115503516</v>
       </c>
       <c r="C7" s="14" t="n">
-        <v>2.844001213689403</v>
+        <v>1.073222713296864</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>9.703072181449262</v>
+        <v>8.001189077243545</v>
       </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
-        <v>2.72522560671845</v>
+        <v>1.030523801090705</v>
       </c>
       <c r="G7" s="13" t="n"/>
       <c r="H7" s="12" t="inlineStr">
@@ -2240,17 +2240,17 @@
         </is>
       </c>
       <c r="I7" s="14" t="n">
-        <v>2.274282554125683</v>
+        <v>0.4963982727724712</v>
       </c>
       <c r="J7" s="14" t="n">
-        <v>2.296414533926163</v>
+        <v>0.5128299628413603</v>
       </c>
       <c r="K7" s="14" t="n">
-        <v>13.13783480376886</v>
+        <v>6.242689743567973</v>
       </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
-        <v>2.2572203961285</v>
+        <v>0.5011767528149951</v>
       </c>
       <c r="N7" s="13" t="n"/>
       <c r="O7" s="13" t="n"/>
@@ -2271,16 +2271,16 @@
         </is>
       </c>
       <c r="B8" s="14" t="n">
-        <v>0.1144526964760178</v>
+        <v>0.2282711709727175</v>
       </c>
       <c r="C8" s="14" t="n">
-        <v>0.1309988390392303</v>
+        <v>0.1043430787734386</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>8.960981046584797</v>
+        <v>8.670575811054526</v>
       </c>
       <c r="E8" s="14" t="n">
-        <v>2.72522560671845</v>
+        <v>1.030523801090705</v>
       </c>
       <c r="F8" s="14" t="n"/>
       <c r="H8" s="12" t="inlineStr">
@@ -2289,16 +2289,16 @@
         </is>
       </c>
       <c r="I8" s="14" t="n">
-        <v>0.1960349207199441</v>
+        <v>0.2444829367845394</v>
       </c>
       <c r="J8" s="14" t="n">
-        <v>0.1053254352962912</v>
+        <v>0.09741931143881596</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>12.38050782994369</v>
+        <v>6.057376353151263</v>
       </c>
       <c r="L8" s="14" t="n">
-        <v>2.2572203961285</v>
+        <v>0.5011767528149951</v>
       </c>
       <c r="M8" s="14" t="n"/>
     </row>
@@ -2408,16 +2408,16 @@
       </c>
       <c r="B14" s="14" t="n"/>
       <c r="C14" s="14" t="n">
-        <v>0.2262904584572695</v>
+        <v>0.1424492013819554</v>
       </c>
       <c r="D14" s="14" t="n">
-        <v>12.08381760429481</v>
+        <v>12.08381760429361</v>
       </c>
       <c r="E14" s="14" t="n">
-        <v>2.701114701647342</v>
+        <v>1.038669115507016</v>
       </c>
       <c r="F14" s="14" t="n">
-        <v>0.1231076356932917</v>
+        <v>0.228271170977066</v>
       </c>
       <c r="H14" s="12" t="inlineStr">
         <is>
@@ -2445,17 +2445,17 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0.2262904584572695</v>
+        <v>0.1424492013819554</v>
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n">
-        <v>12.04577796566226</v>
+        <v>12.04577796566076</v>
       </c>
       <c r="E15" s="14" t="n">
-        <v>2.844001213689614</v>
+        <v>1.073222713288946</v>
       </c>
       <c r="F15" s="14" t="n">
-        <v>0.1309988390130185</v>
+        <v>0.1043430787749007</v>
       </c>
       <c r="H15" s="12" t="inlineStr">
         <is>
@@ -2470,10 +2470,10 @@
         <v>0.465363295794745</v>
       </c>
       <c r="L15" s="14" t="n">
-        <v>0.003367651523479847</v>
+        <v>0.003367651523495589</v>
       </c>
       <c r="M15" s="14" t="n">
-        <v>0.004743235699826326</v>
+        <v>0.004743235699842069</v>
       </c>
     </row>
     <row r="16" ht="15.85" customHeight="1" s="10">
@@ -2483,17 +2483,17 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>12.08381760429481</v>
+        <v>12.08381760429361</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>12.04577796566226</v>
+        <v>12.04577796566076</v>
       </c>
       <c r="D16" s="14" t="n"/>
       <c r="E16" s="14" t="n">
-        <v>12.796691355624</v>
+        <v>12.79669135562373</v>
       </c>
       <c r="F16" s="14" t="n">
-        <v>12.09867764770548</v>
+        <v>12.09867764770441</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
@@ -2521,17 +2521,17 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>2.701114701647342</v>
+        <v>1.038669115507016</v>
       </c>
       <c r="C17" s="14" t="n">
-        <v>2.844001213689614</v>
+        <v>1.073222713288946</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>12.796691355624</v>
+        <v>12.79669135562373</v>
       </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
-        <v>2.725225606724025</v>
+        <v>1.030523801085903</v>
       </c>
       <c r="H17" s="12" t="inlineStr">
         <is>
@@ -2542,14 +2542,14 @@
         <v>0.005820922794185767</v>
       </c>
       <c r="J17" s="14" t="n">
-        <v>0.003367651523479847</v>
+        <v>0.003367651523495589</v>
       </c>
       <c r="K17" s="14" t="n">
         <v>0.4687308738595936</v>
       </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
-        <v>0.002265140801919659</v>
+        <v>0.002265140801941614</v>
       </c>
     </row>
     <row r="18" ht="15.85" customHeight="1" s="10">
@@ -2559,16 +2559,16 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0.1231076356932917</v>
+        <v>0.228271170977066</v>
       </c>
       <c r="C18" s="14" t="n">
-        <v>0.1309988390130185</v>
+        <v>0.1043430787749007</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>12.09867764770548</v>
+        <v>12.09867764770441</v>
       </c>
       <c r="E18" s="14" t="n">
-        <v>2.725225606724025</v>
+        <v>1.030523801085903</v>
       </c>
       <c r="F18" s="14" t="n"/>
       <c r="H18" s="12" t="inlineStr">
@@ -2580,13 +2580,13 @@
         <v>0.005322797304849306</v>
       </c>
       <c r="J18" s="14" t="n">
-        <v>0.004743235699826326</v>
+        <v>0.004743235699842069</v>
       </c>
       <c r="K18" s="14" t="n">
         <v>0.4701064277266727</v>
       </c>
       <c r="L18" s="14" t="n">
-        <v>0.002265140801919659</v>
+        <v>0.002265140801941614</v>
       </c>
       <c r="M18" s="14" t="n"/>
     </row>
@@ -2780,16 +2780,16 @@
       </c>
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n">
-        <v>0.06211140463036885</v>
+        <v>0.1714251235919225</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>8.062588612130609</v>
+        <v>7.95431187669925</v>
       </c>
       <c r="E4" s="14" t="n">
-        <v>2.874882720546051</v>
+        <v>1.135972132034418</v>
       </c>
       <c r="F4" s="14" t="n">
-        <v>0.2071908545984845</v>
+        <v>0.2203516255978594</v>
       </c>
       <c r="G4" s="13" t="n"/>
       <c r="H4" s="12" t="inlineStr">
@@ -2799,16 +2799,16 @@
       </c>
       <c r="I4" s="14" t="n"/>
       <c r="J4" s="14" t="n">
-        <v>0.1030983777729827</v>
+        <v>0.1680232480992382</v>
       </c>
       <c r="K4" s="14" t="n">
-        <v>10.48676195248214</v>
+        <v>6.377219401757972</v>
       </c>
       <c r="L4" s="14" t="n">
-        <v>2.908151926234752</v>
+        <v>0.5100353290390166</v>
       </c>
       <c r="M4" s="14" t="n">
-        <v>0.1404873251914096</v>
+        <v>0.2339177685649756</v>
       </c>
       <c r="N4" s="13" t="n"/>
       <c r="O4" s="13" t="n"/>
@@ -2829,17 +2829,17 @@
         </is>
       </c>
       <c r="B5" s="14" t="n">
-        <v>0.06211140463036885</v>
+        <v>0.1714251235919225</v>
       </c>
       <c r="C5" s="14" t="n"/>
       <c r="D5" s="14" t="n">
-        <v>8.006569333036184</v>
+        <v>7.957869748141968</v>
       </c>
       <c r="E5" s="14" t="n">
-        <v>2.935483613418856</v>
+        <v>1.191056193757402</v>
       </c>
       <c r="F5" s="14" t="n">
-        <v>0.2263305621388694</v>
+        <v>0.1112948041343989</v>
       </c>
       <c r="G5" s="13" t="n"/>
       <c r="H5" s="12" t="inlineStr">
@@ -2848,17 +2848,17 @@
         </is>
       </c>
       <c r="I5" s="14" t="n">
-        <v>0.1030983777729827</v>
+        <v>0.1680232480992382</v>
       </c>
       <c r="J5" s="14" t="n"/>
       <c r="K5" s="14" t="n">
-        <v>10.47856220274357</v>
+        <v>6.396667014244952</v>
       </c>
       <c r="L5" s="14" t="n">
-        <v>3.001984560012908</v>
+        <v>0.525596518780395</v>
       </c>
       <c r="M5" s="14" t="n">
-        <v>0.0838425850827151</v>
+        <v>0.09912344425189006</v>
       </c>
       <c r="N5" s="13" t="n"/>
       <c r="O5" s="13" t="n"/>
@@ -2879,17 +2879,17 @@
         </is>
       </c>
       <c r="B6" s="14" t="n">
-        <v>8.062588612130609</v>
+        <v>7.95431187669925</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>8.006569333036184</v>
+        <v>7.957869748141968</v>
       </c>
       <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n">
-        <v>8.856491601352039</v>
+        <v>7.895715526692852</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>7.859104476890197</v>
+        <v>7.933684952347313</v>
       </c>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="12" t="inlineStr">
@@ -2898,17 +2898,17 @@
         </is>
       </c>
       <c r="I6" s="14" t="n">
-        <v>10.48676195248214</v>
+        <v>6.377219401757972</v>
       </c>
       <c r="J6" s="14" t="n">
-        <v>10.47856220274357</v>
+        <v>6.396667014244952</v>
       </c>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n">
-        <v>11.20511984687745</v>
+        <v>6.589350813815304</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>10.43795098231388</v>
+        <v>6.379621913062743</v>
       </c>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
@@ -2929,17 +2929,17 @@
         </is>
       </c>
       <c r="B7" s="14" t="n">
-        <v>2.874882720546051</v>
+        <v>1.135972132034418</v>
       </c>
       <c r="C7" s="14" t="n">
-        <v>2.935483613418856</v>
+        <v>1.191056193757402</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>8.856491601352039</v>
+        <v>7.895715526692852</v>
       </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n">
-        <v>2.749203952310937</v>
+        <v>1.154526869861</v>
       </c>
       <c r="G7" s="13" t="n"/>
       <c r="H7" s="12" t="inlineStr">
@@ -2948,17 +2948,17 @@
         </is>
       </c>
       <c r="I7" s="14" t="n">
-        <v>2.908151926234752</v>
+        <v>0.5100353290390166</v>
       </c>
       <c r="J7" s="14" t="n">
-        <v>3.001984560012908</v>
+        <v>0.525596518780395</v>
       </c>
       <c r="K7" s="14" t="n">
-        <v>11.20511984687745</v>
+        <v>6.589350813815304</v>
       </c>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n">
-        <v>2.957255371749487</v>
+        <v>0.5099077512191998</v>
       </c>
       <c r="N7" s="13" t="n"/>
       <c r="O7" s="13" t="n"/>
@@ -2979,16 +2979,16 @@
         </is>
       </c>
       <c r="B8" s="14" t="n">
-        <v>0.2071908545984845</v>
+        <v>0.2203516255978594</v>
       </c>
       <c r="C8" s="14" t="n">
-        <v>0.2263305621388694</v>
+        <v>0.1112948041343989</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>7.859104476890197</v>
+        <v>7.933684952347313</v>
       </c>
       <c r="E8" s="14" t="n">
-        <v>2.749203952310937</v>
+        <v>1.154526869861</v>
       </c>
       <c r="F8" s="14" t="n"/>
       <c r="H8" s="12" t="inlineStr">
@@ -2997,16 +2997,16 @@
         </is>
       </c>
       <c r="I8" s="14" t="n">
-        <v>0.1404873251914096</v>
+        <v>0.2339177685649756</v>
       </c>
       <c r="J8" s="14" t="n">
-        <v>0.0838425850827151</v>
+        <v>0.09912344425189006</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>10.43795098231388</v>
+        <v>6.379621913062743</v>
       </c>
       <c r="L8" s="14" t="n">
-        <v>2.957255371749487</v>
+        <v>0.5099077512191998</v>
       </c>
       <c r="M8" s="14" t="n"/>
     </row>
@@ -3116,16 +3116,16 @@
       </c>
       <c r="B14" s="14" t="n"/>
       <c r="C14" s="14" t="n">
-        <v>0.07873614082986091</v>
+        <v>0.1714251235979963</v>
       </c>
       <c r="D14" s="14" t="n">
-        <v>11.69423127716002</v>
+        <v>11.69423127716242</v>
       </c>
       <c r="E14" s="14" t="n">
-        <v>2.874882720540283</v>
+        <v>1.135972132034468</v>
       </c>
       <c r="F14" s="14" t="n">
-        <v>0.2071908546064588</v>
+        <v>0.220351625605056</v>
       </c>
       <c r="H14" s="12" t="inlineStr">
         <is>
@@ -3140,7 +3140,7 @@
         <v>0.3068155992074563</v>
       </c>
       <c r="L14" s="14" t="n">
-        <v>0.00584734573916154</v>
+        <v>0.005847345739131406</v>
       </c>
       <c r="M14" s="14" t="n">
         <v>0.00668911770624058</v>
@@ -3153,17 +3153,17 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0.07873614082986091</v>
+        <v>0.1714251235979963</v>
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n">
-        <v>11.6573241284687</v>
+        <v>11.65732412846972</v>
       </c>
       <c r="E15" s="14" t="n">
-        <v>2.935483613414252</v>
+        <v>1.191056193751623</v>
       </c>
       <c r="F15" s="14" t="n">
-        <v>0.2263305621488368</v>
+        <v>0.1112948041490772</v>
       </c>
       <c r="H15" s="12" t="inlineStr">
         <is>
@@ -3175,13 +3175,13 @@
       </c>
       <c r="J15" s="14" t="n"/>
       <c r="K15" s="14" t="n">
-        <v>0.2983315187058641</v>
+        <v>0.2983315187058467</v>
       </c>
       <c r="L15" s="14" t="n">
         <v>0.003200027864232041</v>
       </c>
       <c r="M15" s="14" t="n">
-        <v>0.00418353106395057</v>
+        <v>0.004183531063985104</v>
       </c>
     </row>
     <row r="16" ht="15.85" customHeight="1" s="10">
@@ -3191,17 +3191,17 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>11.69423127716002</v>
+        <v>11.69423127716242</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>11.6573241284687</v>
+        <v>11.65732412846972</v>
       </c>
       <c r="D16" s="14" t="n"/>
       <c r="E16" s="14" t="n">
-        <v>12.47793868942139</v>
+        <v>12.47793868942164</v>
       </c>
       <c r="F16" s="14" t="n">
-        <v>11.72636687679834</v>
+        <v>11.72636687680021</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
@@ -3212,7 +3212,7 @@
         <v>0.3068155992074563</v>
       </c>
       <c r="J16" s="14" t="n">
-        <v>0.2983315187058641</v>
+        <v>0.2983315187058467</v>
       </c>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n">
@@ -3229,17 +3229,17 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>2.874882720540283</v>
+        <v>1.135972132034468</v>
       </c>
       <c r="C17" s="14" t="n">
-        <v>2.935483613414252</v>
+        <v>1.191056193751623</v>
       </c>
       <c r="D17" s="14" t="n">
-        <v>12.47793868942139</v>
+        <v>12.47793868942164</v>
       </c>
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n">
-        <v>2.749203952297027</v>
+        <v>1.154526869850651</v>
       </c>
       <c r="H17" s="12" t="inlineStr">
         <is>
@@ -3247,7 +3247,7 @@
         </is>
       </c>
       <c r="I17" s="14" t="n">
-        <v>0.00584734573916154</v>
+        <v>0.005847345739131406</v>
       </c>
       <c r="J17" s="14" t="n">
         <v>0.003200027864232041</v>
@@ -3257,7 +3257,7 @@
       </c>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n">
-        <v>0.001997812498847041</v>
+        <v>0.001997812498867454</v>
       </c>
     </row>
     <row r="18" ht="15.85" customHeight="1" s="10">
@@ -3267,16 +3267,16 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0.2071908546064588</v>
+        <v>0.220351625605056</v>
       </c>
       <c r="C18" s="14" t="n">
-        <v>0.2263305621488368</v>
+        <v>0.1112948041490772</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>11.72636687679834</v>
+        <v>11.72636687680021</v>
       </c>
       <c r="E18" s="14" t="n">
-        <v>2.749203952297027</v>
+        <v>1.154526869850651</v>
       </c>
       <c r="F18" s="14" t="n"/>
       <c r="H18" s="12" t="inlineStr">
@@ -3288,13 +3288,13 @@
         <v>0.00668911770624058</v>
       </c>
       <c r="J18" s="14" t="n">
-        <v>0.00418353106395057</v>
+        <v>0.004183531063985104</v>
       </c>
       <c r="K18" s="14" t="n">
         <v>0.3025150120135459</v>
       </c>
       <c r="L18" s="14" t="n">
-        <v>0.001997812498847041</v>
+        <v>0.001997812498867454</v>
       </c>
       <c r="M18" s="14" t="n"/>
     </row>

</xml_diff>